<commit_message>
cleaned data for IT
</commit_message>
<xml_diff>
--- a/Financial_Data/MoneyControl/Companies/IT Services & Consulting/3i Infotech Ltd/Pruned_Excel/Pruned_Cash-flow_combined.xlsx
+++ b/Financial_Data/MoneyControl/Companies/IT Services & Consulting/3i Infotech Ltd/Pruned_Excel/Pruned_Cash-flow_combined.xlsx
@@ -1,132 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Cash Flow of 3i Infotech(in Rs. Cr.)</t>
-  </si>
-  <si>
-    <t>Mar 05</t>
-  </si>
-  <si>
-    <t>Mar 06</t>
-  </si>
-  <si>
-    <t>Mar 07</t>
-  </si>
-  <si>
-    <t>Mar 08</t>
-  </si>
-  <si>
-    <t>Mar 09</t>
-  </si>
-  <si>
-    <t>Mar 10</t>
-  </si>
-  <si>
-    <t>Mar 11</t>
-  </si>
-  <si>
-    <t>Mar 12</t>
-  </si>
-  <si>
-    <t>Mar 13</t>
-  </si>
-  <si>
-    <t>Mar 14</t>
-  </si>
-  <si>
-    <t>Mar 15</t>
-  </si>
-  <si>
-    <t>Mar 16</t>
-  </si>
-  <si>
-    <t>Mar 17</t>
-  </si>
-  <si>
-    <t>Mar 18</t>
-  </si>
-  <si>
-    <t>Mar 19</t>
-  </si>
-  <si>
-    <t>Mar 20</t>
-  </si>
-  <si>
-    <t>Mar 21</t>
-  </si>
-  <si>
-    <t>Mar 22</t>
-  </si>
-  <si>
-    <t>Mar 23</t>
-  </si>
-  <si>
-    <t>Mar 24</t>
-  </si>
-  <si>
-    <t>Net Profit/Loss Before Extraordinary Items And Tax</t>
-  </si>
-  <si>
-    <t>Net CashFlow From Operating Activities</t>
-  </si>
-  <si>
-    <t>Net Cash Used In Investing Activities</t>
-  </si>
-  <si>
-    <t>Net Cash Used From Financing Activities</t>
-  </si>
-  <si>
-    <t>Net Inc/Dec In Cash And Cash Equivalents</t>
-  </si>
-  <si>
-    <t>Cash And Cash Equivalents Begin of Year</t>
-  </si>
-  <si>
-    <t>Cash And Cash Equivalents End Of Year</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -141,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -457,586 +420,622 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Quarter</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Net Profit/Loss Before Extraordinary Items And Tax</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Net CashFlow From Operating Activities</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Net Cash Used In Investing Activities</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Net Cash Used From Financing Activities</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Net Inc/Dec In Cash And Cash Equivalents</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Cash And Cash Equivalents Begin of Year</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Cash And Cash Equivalents End Of Year</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Mar 05</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>19.87</v>
       </c>
-      <c r="C3">
+      <c r="C2" t="n">
         <v>30.62</v>
       </c>
-      <c r="D3">
+      <c r="D2" t="n">
         <v>-58.86</v>
       </c>
-      <c r="E3">
+      <c r="E2" t="n">
         <v>26.5</v>
       </c>
-      <c r="F3">
+      <c r="F2" t="n">
         <v>-1.74</v>
       </c>
-      <c r="G3">
+      <c r="G2" t="n">
         <v>9.66</v>
       </c>
-      <c r="H3">
+      <c r="H2" t="n">
         <v>7.92</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mar 06</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>41</v>
       </c>
-      <c r="C4">
+      <c r="C3" t="n">
         <v>5.16</v>
       </c>
-      <c r="D4">
+      <c r="D3" t="n">
         <v>-74.45999999999999</v>
       </c>
-      <c r="E4">
+      <c r="E3" t="n">
         <v>307.59</v>
       </c>
-      <c r="F4">
+      <c r="F3" t="n">
         <v>238.29</v>
       </c>
-      <c r="G4">
+      <c r="G3" t="n">
         <v>7.92</v>
       </c>
-      <c r="H4">
+      <c r="H3" t="n">
         <v>246.21</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Mar 07</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>51.05</v>
       </c>
-      <c r="C5">
+      <c r="C4" t="n">
         <v>111.26</v>
       </c>
-      <c r="D5">
+      <c r="D4" t="n">
         <v>-418.79</v>
       </c>
-      <c r="E5">
+      <c r="E4" t="n">
         <v>121.78</v>
       </c>
-      <c r="F5">
+      <c r="F4" t="n">
         <v>-185.75</v>
       </c>
-      <c r="G5">
+      <c r="G4" t="n">
         <v>246.21</v>
       </c>
-      <c r="H5">
+      <c r="H4" t="n">
         <v>60.45</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Mar 08</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>104.14</v>
       </c>
-      <c r="C6">
+      <c r="C5" t="n">
         <v>199.67</v>
       </c>
-      <c r="D6">
+      <c r="D5" t="n">
         <v>-764.8</v>
       </c>
-      <c r="E6">
+      <c r="E5" t="n">
         <v>537.35</v>
       </c>
-      <c r="F6">
+      <c r="F5" t="n">
         <v>-27.79</v>
       </c>
-      <c r="G6">
+      <c r="G5" t="n">
         <v>60.45</v>
       </c>
-      <c r="H6">
+      <c r="H5" t="n">
         <v>32.66</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Mar 09</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>161.4</v>
       </c>
-      <c r="C7">
+      <c r="C6" t="n">
         <v>356</v>
       </c>
-      <c r="D7">
+      <c r="D6" t="n">
         <v>-425.97</v>
       </c>
-      <c r="E7">
+      <c r="E6" t="n">
         <v>73.34</v>
       </c>
-      <c r="F7">
+      <c r="F6" t="n">
         <v>3.37</v>
       </c>
-      <c r="G7">
+      <c r="G6" t="n">
         <v>32.66</v>
       </c>
-      <c r="H7">
+      <c r="H6" t="n">
         <v>36.03</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Mar 10</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>136.49</v>
       </c>
-      <c r="C8">
+      <c r="C7" t="n">
         <v>194.8</v>
       </c>
-      <c r="D8">
+      <c r="D7" t="n">
         <v>-386</v>
       </c>
-      <c r="E8">
+      <c r="E7" t="n">
         <v>189.45</v>
       </c>
-      <c r="F8">
+      <c r="F7" t="n">
         <v>-1.75</v>
       </c>
-      <c r="G8">
+      <c r="G7" t="n">
         <v>36.03</v>
       </c>
-      <c r="H8">
+      <c r="H7" t="n">
         <v>34.28</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Mar 11</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>108.15</v>
       </c>
-      <c r="C9">
+      <c r="C8" t="n">
         <v>233.73</v>
       </c>
-      <c r="D9">
+      <c r="D8" t="n">
         <v>-152.96</v>
       </c>
-      <c r="E9">
+      <c r="E8" t="n">
         <v>-21.28</v>
       </c>
-      <c r="F9">
+      <c r="F8" t="n">
         <v>59.49</v>
       </c>
-      <c r="G9">
+      <c r="G8" t="n">
         <v>19.26</v>
       </c>
-      <c r="H9">
+      <c r="H8" t="n">
         <v>78.75</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Mar 12</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>-165.25</v>
       </c>
-      <c r="C10">
+      <c r="C9" t="n">
         <v>-81.36</v>
       </c>
-      <c r="D10">
+      <c r="D9" t="n">
         <v>-15.79</v>
       </c>
-      <c r="E10">
+      <c r="E9" t="n">
         <v>42.79</v>
       </c>
-      <c r="F10">
+      <c r="F9" t="n">
         <v>-54.36</v>
       </c>
-      <c r="G10">
+      <c r="G9" t="n">
         <v>78.75</v>
       </c>
-      <c r="H10">
+      <c r="H9" t="n">
         <v>24.39</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Mar 13</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>-379.45</v>
       </c>
-      <c r="C11">
+      <c r="C10" t="n">
         <v>36.45</v>
       </c>
-      <c r="D11">
+      <c r="D10" t="n">
         <v>-39.79</v>
       </c>
-      <c r="E11">
+      <c r="E10" t="n">
         <v>-15.03</v>
       </c>
-      <c r="F11">
+      <c r="F10" t="n">
         <v>-18.37</v>
       </c>
-      <c r="G11">
+      <c r="G10" t="n">
         <v>24.39</v>
       </c>
-      <c r="H11">
+      <c r="H10" t="n">
         <v>6.02</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Mar 14</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>-417.92</v>
       </c>
-      <c r="C12">
+      <c r="C11" t="n">
         <v>-72.54000000000001</v>
       </c>
-      <c r="D12">
+      <c r="D11" t="n">
         <v>2.01</v>
       </c>
-      <c r="E12">
+      <c r="E11" t="n">
         <v>77.52</v>
       </c>
-      <c r="F12">
+      <c r="F11" t="n">
         <v>6.99</v>
       </c>
-      <c r="G12">
+      <c r="G11" t="n">
         <v>6.02</v>
       </c>
-      <c r="H12">
+      <c r="H11" t="n">
         <v>13.01</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Mar 15</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>-343.56</v>
       </c>
-      <c r="C13">
+      <c r="C12" t="n">
         <v>73.98999999999999</v>
       </c>
-      <c r="D13">
+      <c r="D12" t="n">
         <v>-3.19</v>
       </c>
-      <c r="E13">
+      <c r="E12" t="n">
         <v>-79.31999999999999</v>
       </c>
-      <c r="F13">
+      <c r="F12" t="n">
         <v>-8.52</v>
       </c>
-      <c r="G13">
+      <c r="G12" t="n">
         <v>13.01</v>
       </c>
-      <c r="H13">
+      <c r="H12" t="n">
         <v>4.49</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Mar 16</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>-448</v>
       </c>
-      <c r="C14">
+      <c r="C13" t="n">
         <v>35.39</v>
       </c>
-      <c r="D14">
+      <c r="D13" t="n">
         <v>2.76</v>
       </c>
-      <c r="E14">
+      <c r="E13" t="n">
         <v>-25.33</v>
       </c>
-      <c r="F14">
+      <c r="F13" t="n">
         <v>12.82</v>
       </c>
-      <c r="G14">
+      <c r="G13" t="n">
         <v>7.83</v>
       </c>
-      <c r="H14">
+      <c r="H13" t="n">
         <v>20.65</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Mar 17</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
         <v>91.09</v>
       </c>
-      <c r="C15">
+      <c r="C14" t="n">
         <v>113.86</v>
       </c>
-      <c r="D15">
+      <c r="D14" t="n">
         <v>16.61</v>
       </c>
-      <c r="E15">
+      <c r="E14" t="n">
         <v>-56.31</v>
       </c>
-      <c r="F15">
+      <c r="F14" t="n">
         <v>74.16</v>
       </c>
-      <c r="G15">
+      <c r="G14" t="n">
         <v>20.65</v>
       </c>
-      <c r="H15">
+      <c r="H14" t="n">
         <v>94.81</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Mar 18</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
         <v>-86.70999999999999</v>
       </c>
-      <c r="C16">
+      <c r="C15" t="n">
         <v>82.2</v>
       </c>
-      <c r="D16">
+      <c r="D15" t="n">
         <v>1.29</v>
       </c>
-      <c r="E16">
+      <c r="E15" t="n">
         <v>-146.08</v>
       </c>
-      <c r="F16">
+      <c r="F15" t="n">
         <v>-62.59</v>
       </c>
-      <c r="G16">
+      <c r="G15" t="n">
         <v>94.81</v>
       </c>
-      <c r="H16">
+      <c r="H15" t="n">
         <v>32.22</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Mar 19</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
         <v>250.85</v>
       </c>
-      <c r="C17">
+      <c r="C16" t="n">
         <v>86.52</v>
       </c>
-      <c r="D17">
+      <c r="D16" t="n">
         <v>2.64</v>
       </c>
-      <c r="E17">
+      <c r="E16" t="n">
         <v>-41.91</v>
       </c>
-      <c r="F17">
+      <c r="F16" t="n">
         <v>47.25</v>
       </c>
-      <c r="G17">
+      <c r="G16" t="n">
         <v>32.22</v>
       </c>
-      <c r="H17">
+      <c r="H16" t="n">
         <v>79.47</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mar 20</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
         <v>127.96</v>
       </c>
-      <c r="C18">
+      <c r="C17" t="n">
         <v>103.84</v>
       </c>
-      <c r="D18">
+      <c r="D17" t="n">
         <v>16.68</v>
       </c>
-      <c r="E18">
+      <c r="E17" t="n">
         <v>-132.75</v>
       </c>
-      <c r="F18">
+      <c r="F17" t="n">
         <v>-12.23</v>
       </c>
-      <c r="G18">
+      <c r="G17" t="n">
         <v>79.47</v>
       </c>
-      <c r="H18">
+      <c r="H17" t="n">
         <v>67.23999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Mar 21</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
         <v>324.56</v>
       </c>
-      <c r="C19">
+      <c r="C18" t="n">
         <v>388.69</v>
       </c>
-      <c r="D19">
+      <c r="D18" t="n">
         <v>561.6</v>
       </c>
-      <c r="E19">
+      <c r="E18" t="n">
         <v>-380.01</v>
       </c>
-      <c r="F19">
+      <c r="F18" t="n">
         <v>570.28</v>
       </c>
-      <c r="G19">
+      <c r="G18" t="n">
         <v>67.25</v>
       </c>
-      <c r="H19">
+      <c r="H18" t="n">
         <v>637.53</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Mar 22</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
         <v>8.43</v>
       </c>
-      <c r="C20">
+      <c r="C19" t="n">
         <v>-57.44</v>
       </c>
-      <c r="D20">
+      <c r="D19" t="n">
         <v>10.09</v>
       </c>
-      <c r="E20">
+      <c r="E19" t="n">
         <v>-504.03</v>
       </c>
-      <c r="F20">
+      <c r="F19" t="n">
         <v>-551.38</v>
       </c>
-      <c r="G20">
+      <c r="G19" t="n">
         <v>637.53</v>
       </c>
-      <c r="H20">
+      <c r="H19" t="n">
         <v>86.15000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21">
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Mar 23</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
         <v>52.25</v>
       </c>
-      <c r="C21">
+      <c r="C20" t="n">
         <v>108</v>
       </c>
-      <c r="D21">
+      <c r="D20" t="n">
         <v>-105.15</v>
       </c>
-      <c r="E21">
+      <c r="E20" t="n">
         <v>-48.48</v>
       </c>
-      <c r="F21">
+      <c r="F20" t="n">
         <v>-45.63</v>
       </c>
-      <c r="G21">
+      <c r="G20" t="n">
         <v>86.14</v>
       </c>
-      <c r="H21">
+      <c r="H20" t="n">
         <v>40.51</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22">
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Mar 24</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
         <v>-818.63</v>
       </c>
-      <c r="C22">
+      <c r="C21" t="n">
         <v>14.63</v>
       </c>
-      <c r="D22">
+      <c r="D21" t="n">
         <v>-10.34</v>
       </c>
-      <c r="E22">
+      <c r="E21" t="n">
         <v>-16.05</v>
       </c>
-      <c r="F22">
+      <c r="F21" t="n">
         <v>-11.76</v>
       </c>
-      <c r="G22">
+      <c r="G21" t="n">
         <v>40.51</v>
       </c>
-      <c r="H22">
+      <c r="H21" t="n">
         <v>28.75</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>